<commit_message>
change some feature in monitoring revamp klasifikasi text ubah gitignore
</commit_message>
<xml_diff>
--- a/data_sample_sedang.xlsx
+++ b/data_sample_sedang.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Python Projects\env1\Projects\social-media-data-analysist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4E6DCB-208C-4AF5-8745-23CF0790819C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC59EC9-EFE0-4294-B9F5-B55F3286189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6510" uniqueCount="2061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6510" uniqueCount="2062">
   <si>
     <t>UUID</t>
   </si>
@@ -6203,6 +6203,9 @@
   </si>
   <si>
     <t>https://instagram.com/p/DBL1DvSSonS/</t>
+  </si>
+  <si>
+    <t>Lowongan baru, gaji berkisar 10 juta silakan melamar\u2757 Perhatian : Ketika melamar lowongan kerja, anda tidak boleh membayar sejumlah uang kepada seseorang/ perusahaan. Jika ada yang meminta, Tolak Saja! Kemungkinan besar itu adalah sebuah penipuan. Belakangan ini sering terjadi penipuan kepada calon pencari kerja. Selalu berhati-hati dan waspada terhadap segala bentuk penipuan! . . #lokergresik #lokergresikterbaru #lowongangresik #lowongankerjagresik #infogresik #gresikhits #infokerjagresik #infolokergresik #lowkergresik #likeforlikes #lokerjatim #lokerjawatimur #lokerterbaru #infoloker #lokerfreshgraduate #lokersma #infolokerterupdate #informasilowongankerja #lowongankerja #openrecruitment #hiring #lb #loker2024 #infolowker #jobvacancy</t>
   </si>
 </sst>
 </file>
@@ -6584,8 +6587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
-      <selection activeCell="E461" sqref="E461:E500"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="H230" sqref="H230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20820,7 +20823,7 @@
         <v>909</v>
       </c>
       <c r="H230" t="s">
-        <v>910</v>
+        <v>2061</v>
       </c>
       <c r="J230" t="s">
         <v>30</v>

</xml_diff>